<commit_message>
add/remove officer from access
- dataset
- datatable
- datatablecolumn
</commit_message>
<xml_diff>
--- a/src/test/java/sg/gov/csit/datacatalogue/dcms/datatable/testfiles/test.xlsx
+++ b/src/test/java/sg/gov/csit/datacatalogue/dcms/datatable/testfiles/test.xlsx
@@ -28,9 +28,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Dulce</t>
-  </si>
-  <si>
     <t>Abril</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>Singapore</t>
+  </si>
+  <si>
+    <t>``~!@#$%^&amp;*()''/'"".;:&gt;&lt;</t>
   </si>
 </sst>
 </file>
@@ -123,9 +123,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -136,6 +136,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF000000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,12 +164,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +468,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -473,13 +480,13 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -494,24 +501,24 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="13.5">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
       <c r="F2">
         <v>32</v>
@@ -528,16 +535,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
       </c>
       <c r="F3">
         <v>25</v>
@@ -554,16 +561,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
       </c>
       <c r="F4">
         <v>36</v>
@@ -580,16 +587,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="F5">
         <v>25</v>
@@ -606,16 +613,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
       <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="F6">
         <v>58</v>
@@ -632,16 +639,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7">
         <v>24</v>
@@ -658,16 +665,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <v>56</v>
@@ -684,16 +691,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="F9">
         <v>27</v>
@@ -710,16 +717,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
       <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="F10">
         <v>40</v>
@@ -736,16 +743,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="F11">
         <v>55</v>

</xml_diff>